<commit_message>
revised all rating curves and scripts for Lake Hodges sites
</commit_message>
<xml_diff>
--- a/LakeHodges/Equipment Settings.xlsx
+++ b/LakeHodges/Equipment Settings.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23328"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alex.messina\Documents\GitHub\Sutron_scripts\LakeHodges\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0A88250-BEFC-44B8-AAAD-C9A56DBFE202}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9120" activeTab="2"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sutron" sheetId="4" r:id="rId1"/>
@@ -266,7 +267,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -357,7 +358,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="2" name="EsriDoNotEdit"/>
+        <xdr:cNvPr id="2" name="EsriDoNotEdit">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr/>
       </xdr:nvSpPr>
       <xdr:spPr>
@@ -696,32 +703,32 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="L12" sqref="L12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.5546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.21875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.44140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.44140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.88671875" customWidth="1"/>
-    <col min="8" max="8" width="14.109375" customWidth="1"/>
-    <col min="9" max="9" width="11.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="14.85546875" customWidth="1"/>
+    <col min="8" max="8" width="14.140625" customWidth="1"/>
+    <col min="9" max="9" width="12.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
       <c r="B2" s="4" t="s">
         <v>36</v>
@@ -744,7 +751,7 @@
       <c r="H2" s="3"/>
       <c r="I2" s="3"/>
     </row>
-    <row r="3" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
@@ -773,37 +780,37 @@
         <v>49</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>8</v>
       </c>
@@ -816,7 +823,7 @@
       <c r="H10" s="3"/>
       <c r="I10" s="3"/>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>9</v>
       </c>
@@ -839,7 +846,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>10</v>
       </c>
@@ -862,7 +869,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>11</v>
       </c>
@@ -885,7 +892,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>12</v>
       </c>
@@ -908,7 +915,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>13</v>
       </c>
@@ -931,7 +938,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>14</v>
       </c>
@@ -954,7 +961,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>15</v>
       </c>
@@ -977,7 +984,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>16</v>
       </c>
@@ -1002,7 +1009,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>17</v>
       </c>
@@ -1031,30 +1038,30 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:S18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="S5" sqref="S5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.5546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.6640625" customWidth="1"/>
-    <col min="4" max="4" width="12.21875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.44140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.44140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.7109375" customWidth="1"/>
+    <col min="4" max="4" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.42578125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="15" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="15.21875" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="13.88671875" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="19.6640625" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="17.21875" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="12.5546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="19.7109375" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="12.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1062,7 +1069,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="2" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:19" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -1121,12 +1128,12 @@
         <v>76</v>
       </c>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -1185,7 +1192,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -1202,7 +1209,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -1219,7 +1226,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -1236,7 +1243,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -1253,12 +1260,12 @@
         <v>23</v>
       </c>
     </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>9</v>
       </c>
@@ -1275,7 +1282,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>10</v>
       </c>
@@ -1292,7 +1299,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>11</v>
       </c>
@@ -1309,7 +1316,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>12</v>
       </c>
@@ -1326,7 +1333,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>13</v>
       </c>
@@ -1343,7 +1350,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>14</v>
       </c>
@@ -1360,7 +1367,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>15</v>
       </c>
@@ -1377,7 +1384,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>16</v>
       </c>
@@ -1394,7 +1401,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>17</v>
       </c>
@@ -1417,30 +1424,30 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:E18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.5546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.21875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.44140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.44140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -1457,12 +1464,12 @@
         <v>32</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -1476,7 +1483,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -1490,7 +1497,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -1504,7 +1511,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -1518,7 +1525,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -1532,12 +1539,12 @@
         <v>33</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>9</v>
       </c>
@@ -1551,7 +1558,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>10</v>
       </c>
@@ -1565,7 +1572,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>11</v>
       </c>
@@ -1579,7 +1586,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>12</v>
       </c>
@@ -1593,7 +1600,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>13</v>
       </c>
@@ -1607,7 +1614,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>14</v>
       </c>
@@ -1621,7 +1628,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>15</v>
       </c>
@@ -1635,7 +1642,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>16</v>
       </c>
@@ -1649,7 +1656,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>17</v>
       </c>
@@ -1669,12 +1676,12 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>